<commit_message>
add'd delete function -> fix read on qryname box
</commit_message>
<xml_diff>
--- a/EmailSqlResults/txtQueryName_1.xlsx
+++ b/EmailSqlResults/txtQueryName_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -48,7 +48,7 @@
     <t>To</t>
   </si>
   <si>
-    <t>Cynthia Nonnenmacher</t>
+    <t>Dani Feng</t>
   </si>
   <si>
     <t>Secondary</t>
@@ -57,232 +57,178 @@
     <t>Input</t>
   </si>
   <si>
-    <t>ActivityLog</t>
-  </si>
-  <si>
-    <t>ControlNo</t>
-  </si>
-  <si>
-    <t>EntityName</t>
-  </si>
-  <si>
-    <t>NovoCure Ltd.</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>IPO</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>The company registered for a USD 300M IPO on August 31, 2015.</t>
-  </si>
-  <si>
-    <t>DeptAssigned</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>UserAssigned</t>
-  </si>
-  <si>
-    <t>CYN</t>
-  </si>
-  <si>
-    <t>PerformedBy</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>Person</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>SiteId</t>
-  </si>
-  <si>
-    <t>IsDeleted</t>
-  </si>
-  <si>
-    <t>Zhuojun Xian</t>
-  </si>
-  <si>
-    <t>Goldman Sachs Private Equity Group</t>
-  </si>
-  <si>
-    <t>DISCUPD</t>
-  </si>
-  <si>
-    <t>FUNDR</t>
-  </si>
-  <si>
-    <t>ZX</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Rodnie Tauro</t>
-  </si>
-  <si>
-    <t>Primary</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>InputBy</t>
+  </si>
+  <si>
+    <t>dani.feng@dowjones.com</t>
+  </si>
+  <si>
+    <t>InputDate</t>
+  </si>
+  <si>
+    <t>EditBy</t>
+  </si>
+  <si>
+    <t>EditDate</t>
+  </si>
+  <si>
+    <t>SendMail</t>
+  </si>
+  <si>
+    <t>SendEmail</t>
+  </si>
+  <si>
+    <t>Irene Yao</t>
+  </si>
+  <si>
+    <t>PersonID</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Voog</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Romain</t>
+  </si>
+  <si>
+    <t>Prefix1</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>EntityId</t>
+  </si>
+  <si>
+    <t>HomeEmailAddr</t>
+  </si>
+  <si>
+    <t>romain.voog@global-fashion-group.com</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>President &amp; Managing Director, Amazon; Managing Director, Carrefour; Project Leader, The Boston Consulting Group; Consultant, Bain &amp; Co.</t>
+  </si>
+  <si>
+    <t>irene.yao@dowjones.com</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Master's, Business &amp; Economics, Ecole Centrale de Paris</t>
+  </si>
+  <si>
+    <t>Jiayao Zhu</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Manager, R&amp;D, NinePoint Medical Inc.; Manager, R&amp;D, AngioDynamics</t>
+  </si>
+  <si>
+    <t>jiayao.zhu@dowjones.com</t>
+  </si>
+  <si>
+    <t>BS, Plastics Engineering, University of Massachusetts</t>
+  </si>
+  <si>
+    <t>Ivy Guo</t>
+  </si>
+  <si>
+    <t>Beaver</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>ivy.guo@dowjones.com</t>
+  </si>
+  <si>
+    <t>Erpelding</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>jone@nusourcefinancial.com</t>
+  </si>
+  <si>
+    <t>Bachelor's, Business, Management, Marketing &amp; Related Support Services, Minnesota State University</t>
+  </si>
+  <si>
+    <t>Medeiros</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>emedeiros@sunbehavioral.com</t>
+  </si>
+  <si>
+    <t>Managing Partner, Galeao Partners; Principal, New MainStream Capital; Investment Banker, Goldman Sachs &amp; Co.</t>
+  </si>
+  <si>
+    <t>FCCode</t>
+  </si>
+  <si>
+    <t>Whitelock</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>BSc, Applied Physics, Dublin City University</t>
+  </si>
+  <si>
+    <t>Nealon</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>terry.nealon@fishtree.com</t>
+  </si>
+  <si>
+    <t>EVP &amp; GM, Houghton Mifflin Harcourt; Director, Sales, Riverdeep</t>
+  </si>
+  <si>
+    <t>MBA, University College Dublin; Master, University College Dublin; Bachelor, Commerce, National University of Ireland</t>
   </si>
   <si>
     <t>Edit</t>
   </si>
   <si>
-    <t xml:space="preserve"> // empl per LinkedIn, please check if June 2013 is seed or indi NK 4/4/2014 // PVAL:  17.82 // Descry: United States_First Round_Consumer Information Services_Consumer Services</t>
-  </si>
-  <si>
-    <t>// empl per LinkedIn, please check if June 2013 is seed or indi NK 4/4/2014 // PVAL:  17.82 // Descry: United States_First Round_Consumer Information Services_Consumer Services//LM Berg: 1p, gen vm [RT9/1/15]</t>
-  </si>
-  <si>
-    <t>EditBy</t>
-  </si>
-  <si>
-    <t>rodnie.tauro@dowjones.com</t>
-  </si>
-  <si>
-    <t>Mine Ekim</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> //  // PVAL: 42240 12.16 // Descry: United States_First Round_Medical Software and Information Services_Healthcare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//  // PVAL: 42240 12.16 // Descry: United States_First Round_Medical Software and Information Services_Healthcare // SE Tony Coco: 1p, sent direct em tony.coco@bluestrataemr.com [MIE 9/1/2015] // </t>
-  </si>
-  <si>
-    <t>mine.ekim@dowjones.com</t>
-  </si>
-  <si>
-    <t>Ruoying Wang</t>
-  </si>
-  <si>
-    <t>The Network Inc.</t>
-  </si>
-  <si>
-    <t>NewCoRe</t>
-  </si>
-  <si>
-    <t>BUY</t>
-  </si>
-  <si>
-    <t>RYW</t>
-  </si>
-  <si>
-    <t>Armin Toor</t>
-  </si>
-  <si>
-    <t>Luxury Hues Group Consultancy (India) Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>NEWSUPD</t>
-  </si>
-  <si>
-    <t>per VC Circle 9/1/15 ded 60M 1st round not confirmed, close 9/1/15, investors=Reliance+Individual Investor Ravi Viswanathan, news=Y. Pls confirm that Ravi Viswanathan invested in round [AT 9/1/15]</t>
-  </si>
-  <si>
-    <t>VC</t>
-  </si>
-  <si>
-    <t>ART</t>
-  </si>
-  <si>
-    <t>Ivy Guo</t>
-  </si>
-  <si>
-    <t>Gas &amp; Alloy Supply Company</t>
-  </si>
-  <si>
-    <t>ACQ</t>
-  </si>
-  <si>
-    <t>GI</t>
-  </si>
-  <si>
-    <t>Xizhu Xiao</t>
-  </si>
-  <si>
-    <t>Beijing Chedao Network Technology Co. Ltd.</t>
-  </si>
-  <si>
-    <t>XZX</t>
-  </si>
-  <si>
-    <t>Zainab Bisiolu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> //  // PVAL: 42237 15.8 // Descry: United States_First Round_Healthcare Services_Healthcare</t>
-  </si>
-  <si>
-    <t>REFUSAL//  // PVAL: 42237 15.8 // webup</t>
-  </si>
-  <si>
-    <t>zainab.bisiolu@dowjones.c</t>
-  </si>
-  <si>
-    <t>Valerie Foo</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>//  // PVAL: 42243  // Descry: Not PVal Round Type</t>
-  </si>
-  <si>
-    <t>//  // PVAL: 42243  // Descry: Not PVal Round Type // RE Horne: info ok/fine as-is on profile, will treat as cnfmd [VF 9/1/2015]</t>
-  </si>
-  <si>
-    <t>VF</t>
-  </si>
-  <si>
-    <t>valerie.foo@dowjones.com</t>
-  </si>
-  <si>
-    <t>Aberdeen Asset Management PLC</t>
-  </si>
-  <si>
-    <t>MediBeacon LLC</t>
-  </si>
-  <si>
-    <t>MediBeacon Inc.</t>
-  </si>
-  <si>
-    <t>BIG ROUND: US 22.4M //  // PVAL: 42244 44.4 // Descry: United States_Second Round_Medical Devices and Equipment_Healthcare</t>
-  </si>
-  <si>
-    <t>BIG ROUND: US 22.4M //  // PVAL: 42244 44.4 // Descry: United States_Second Round_Medical Devices and Equipment_Healthcare // SE  Terence Stern: 1p, sent direct em stern@medibeacon.com and cc'd Steven J. Hanley - hanley@medibeacon.com [MIE 9/1/2015] //</t>
-  </si>
-  <si>
-    <t>Fliptop Inc.</t>
-  </si>
-  <si>
-    <t>Irene Yao</t>
-  </si>
-  <si>
-    <t>CytomX Therapeutics Inc.</t>
-  </si>
-  <si>
-    <t>IY</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>irene.yao@dowjones.com</t>
-  </si>
-  <si>
-    <t>Backyard Leisure Holdings LLC</t>
+    <t>Managing Director &amp; CFO, Kupishoes LLC; Investment Professional, Morgan Stanley Private Equity</t>
   </si>
 </sst>
 </file>
@@ -318,8 +264,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -662,7 +609,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -671,7 +618,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -683,15 +630,15 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <v>1857196</v>
-      </c>
-      <c r="J2">
-        <v>1857196</v>
+        <v>1885344</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -700,7 +647,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -709,18 +656,18 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>1857196</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
+        <v>1885344</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -729,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -741,7 +688,7 @@
         <v>17</v>
       </c>
       <c r="H4">
-        <v>1857196</v>
+        <v>1885344</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -749,7 +696,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -758,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -770,15 +717,15 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <v>1857196</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
+        <v>1885344</v>
+      </c>
+      <c r="J5" s="2">
+        <v>42106.905474537038</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -787,7 +734,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -796,18 +743,18 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6">
-        <v>1857196</v>
+        <v>1885344</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -816,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -825,18 +772,18 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H7">
-        <v>1857196</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
+        <v>1885344</v>
+      </c>
+      <c r="J7" s="2">
+        <v>42106.90552083333</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -845,7 +792,7 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -854,18 +801,18 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8">
-        <v>1857196</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
+        <v>1885344</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -874,7 +821,7 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>358552</v>
+        <v>661798</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -883,27 +830,27 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H9">
-        <v>1857196</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
+        <v>1885344</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10">
-        <v>358552</v>
+        <v>661797</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -912,27 +859,27 @@
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>1857196</v>
-      </c>
-      <c r="J10" t="s">
-        <v>29</v>
+        <v>1885343</v>
+      </c>
+      <c r="J10">
+        <v>1885343</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11">
-        <v>358552</v>
+        <v>661797</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -941,27 +888,27 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H11">
-        <v>1857196</v>
-      </c>
-      <c r="J11">
-        <v>650289</v>
+        <v>1885343</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>42248.710196759261</v>
+        <v>42108</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12">
-        <v>358552</v>
+        <v>661797</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -970,27 +917,27 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H12">
-        <v>1857196</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
+        <v>1885343</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -999,56 +946,56 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="H13">
-        <v>1857170</v>
-      </c>
-      <c r="J13">
-        <v>1857170</v>
+        <v>1885343</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>661797</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14">
-        <v>73163</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
       <c r="H14">
-        <v>1857170</v>
-      </c>
-      <c r="J14" t="s">
-        <v>33</v>
+        <v>1885343</v>
+      </c>
+      <c r="J14">
+        <v>661797</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1057,10 +1004,10 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="H15">
-        <v>1857170</v>
+        <v>1885343</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
@@ -1068,16 +1015,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1086,27 +1033,27 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H16">
-        <v>1857170</v>
+        <v>1885343</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1115,27 +1062,27 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H17">
-        <v>1857170</v>
+        <v>1885343</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1144,27 +1091,27 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H18">
-        <v>1857170</v>
-      </c>
-      <c r="J18" t="s">
-        <v>27</v>
+        <v>1885343</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1173,10 +1120,10 @@
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H19">
-        <v>1857170</v>
+        <v>1885343</v>
       </c>
       <c r="J19" t="s">
         <v>37</v>
@@ -1184,16 +1131,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>42248.316736111112</v>
+        <v>42108</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20">
-        <v>73163</v>
+        <v>661797</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1202,207 +1149,201 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H20">
-        <v>1857170</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
+        <v>1885343</v>
+      </c>
+      <c r="J20" s="2">
+        <v>42106.900231481479</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>42248.752280092594</v>
+        <v>42108</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>651232</v>
+        <v>661797</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H21">
-        <v>1856361</v>
-      </c>
-      <c r="I21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" t="s">
-        <v>42</v>
+        <v>1885343</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>42248.752280092594</v>
+        <v>42108</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>651232</v>
+        <v>661797</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="H22">
-        <v>1856361</v>
-      </c>
-      <c r="J22" t="s">
-        <v>44</v>
+        <v>1885343</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>42248.692013888889</v>
+        <v>42108</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>661797</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23">
+        <v>1885343</v>
+      </c>
+      <c r="J23" t="s">
         <v>39</v>
-      </c>
-      <c r="D23">
-        <v>665706</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23">
-        <v>1857082</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>42248.692013888889</v>
+        <v>42108</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D24">
-        <v>665706</v>
+        <v>661795</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24">
-        <v>1857082</v>
-      </c>
-      <c r="J24" t="s">
-        <v>27</v>
+        <v>1885342</v>
+      </c>
+      <c r="J24">
+        <v>1885342</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>42248.692013888889</v>
+        <v>42108</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D25">
-        <v>665706</v>
+        <v>661795</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="H25">
-        <v>1857082</v>
+        <v>1885342</v>
       </c>
       <c r="J25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>42248.692013888889</v>
+        <v>42108</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26">
-        <v>665706</v>
+        <v>661795</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H26">
-        <v>1857082</v>
-      </c>
-      <c r="J26">
-        <v>705499</v>
+        <v>1885342</v>
+      </c>
+      <c r="J26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D27">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1411,27 +1352,27 @@
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="H27">
-        <v>1857151</v>
-      </c>
-      <c r="J27">
-        <v>1857151</v>
+        <v>1885342</v>
+      </c>
+      <c r="J27" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D28">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -1440,27 +1381,27 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H28">
-        <v>1857151</v>
-      </c>
-      <c r="J28" t="s">
-        <v>50</v>
+        <v>1885342</v>
+      </c>
+      <c r="J28">
+        <v>661795</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D29">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1469,27 +1410,27 @@
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H29">
-        <v>1857151</v>
+        <v>1885342</v>
       </c>
       <c r="J29" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D30">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -1498,27 +1439,27 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H30">
-        <v>1857151</v>
+        <v>1885342</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D31">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1527,27 +1468,27 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H31">
-        <v>1857151</v>
-      </c>
-      <c r="J31" t="s">
-        <v>53</v>
+        <v>1885342</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D32">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1556,27 +1497,27 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H32">
-        <v>1857151</v>
+        <v>1885342</v>
       </c>
       <c r="J32" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D33">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -1585,27 +1526,27 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H33">
-        <v>1857151</v>
-      </c>
-      <c r="J33" t="s">
-        <v>37</v>
+        <v>1885342</v>
+      </c>
+      <c r="J33" s="2">
+        <v>42106.872986111113</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>42248.141909722224</v>
+        <v>42108</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D34">
-        <v>665972</v>
+        <v>661795</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1614,10 +1555,10 @@
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H34">
-        <v>1857151</v>
+        <v>1885342</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -1625,16 +1566,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D35">
-        <v>665991</v>
+        <v>661795</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -1643,27 +1584,27 @@
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H35">
-        <v>1857182</v>
-      </c>
-      <c r="J35">
-        <v>1857182</v>
+        <v>1885342</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D36">
-        <v>665991</v>
+        <v>661795</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1672,27 +1613,27 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="H36">
-        <v>1857182</v>
+        <v>1885342</v>
       </c>
       <c r="J36" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1701,27 +1642,27 @@
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H37">
-        <v>1857182</v>
-      </c>
-      <c r="J37" t="s">
-        <v>56</v>
+        <v>1885341</v>
+      </c>
+      <c r="J37">
+        <v>1885341</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
       </c>
       <c r="D38">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1730,27 +1671,27 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H38">
-        <v>1857182</v>
+        <v>1885341</v>
       </c>
       <c r="J38" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
       </c>
       <c r="D39">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1759,27 +1700,27 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H39">
-        <v>1857182</v>
+        <v>1885341</v>
       </c>
       <c r="J39" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
       </c>
       <c r="D40">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1788,27 +1729,27 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H40">
-        <v>1857182</v>
+        <v>1885341</v>
       </c>
       <c r="J40" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1817,27 +1758,27 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H41">
-        <v>1857182</v>
-      </c>
-      <c r="J41" t="s">
-        <v>59</v>
+        <v>1885341</v>
+      </c>
+      <c r="J41">
+        <v>661796</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1846,27 +1787,27 @@
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H42">
-        <v>1857182</v>
+        <v>1885341</v>
       </c>
       <c r="J42" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1875,27 +1816,27 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H43">
-        <v>1857182</v>
-      </c>
-      <c r="J43" t="s">
-        <v>37</v>
+        <v>1885341</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1904,27 +1845,27 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H44">
-        <v>1857182</v>
-      </c>
-      <c r="J44">
-        <v>705824</v>
+        <v>1885341</v>
+      </c>
+      <c r="J44" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>42248.563877314817</v>
+        <v>42108</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
       </c>
       <c r="D45">
-        <v>665991</v>
+        <v>661796</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1933,27 +1874,27 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H45">
-        <v>1857182</v>
-      </c>
-      <c r="J45" t="b">
-        <v>0</v>
+        <v>1885341</v>
+      </c>
+      <c r="J45" s="2">
+        <v>42106.871134259258</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1962,27 +1903,27 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H46">
-        <v>1857206</v>
-      </c>
-      <c r="J46">
-        <v>1857206</v>
+        <v>1885341</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
       </c>
       <c r="D47">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1991,27 +1932,27 @@
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H47">
-        <v>1857206</v>
-      </c>
-      <c r="J47" t="s">
-        <v>61</v>
+        <v>1885341</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
       </c>
       <c r="D48">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2020,27 +1961,27 @@
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H48">
-        <v>1857206</v>
-      </c>
-      <c r="J48" t="s">
-        <v>51</v>
+        <v>1885340</v>
+      </c>
+      <c r="J48">
+        <v>1885340</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
       </c>
       <c r="D49">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2049,27 +1990,27 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H49">
-        <v>1857206</v>
+        <v>1885340</v>
       </c>
       <c r="J49" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>11</v>
       </c>
       <c r="D50">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2078,27 +2019,27 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H50">
-        <v>1857206</v>
+        <v>1885340</v>
       </c>
       <c r="J50" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
       </c>
       <c r="D51">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2107,27 +2048,27 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H51">
-        <v>1857206</v>
+        <v>1885340</v>
       </c>
       <c r="J51" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
       </c>
       <c r="D52">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2136,27 +2077,27 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H52">
-        <v>1857206</v>
-      </c>
-      <c r="J52" t="s">
-        <v>37</v>
+        <v>1885340</v>
+      </c>
+      <c r="J52">
+        <v>661796</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>42248.818252314813</v>
+        <v>42108</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
       </c>
       <c r="D53">
-        <v>666006</v>
+        <v>661796</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2165,27 +2106,27 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H53">
-        <v>1857206</v>
-      </c>
-      <c r="J53" t="b">
-        <v>0</v>
+        <v>1885340</v>
+      </c>
+      <c r="J53" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D54">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2197,24 +2138,24 @@
         <v>14</v>
       </c>
       <c r="H54">
-        <v>1857209</v>
-      </c>
-      <c r="J54">
-        <v>1857209</v>
+        <v>1885340</v>
+      </c>
+      <c r="J54" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D55">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2223,27 +2164,27 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H55">
-        <v>1857209</v>
-      </c>
-      <c r="J55" t="s">
-        <v>65</v>
+        <v>1885340</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D56">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2255,24 +2196,24 @@
         <v>17</v>
       </c>
       <c r="H56">
-        <v>1857209</v>
+        <v>1885340</v>
       </c>
       <c r="J56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D57">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2281,27 +2222,27 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H57">
-        <v>1857209</v>
-      </c>
-      <c r="J57" t="s">
-        <v>58</v>
+        <v>1885340</v>
+      </c>
+      <c r="J57" s="2">
+        <v>42106.86954861111</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D58">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -2310,27 +2251,27 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H58">
-        <v>1857209</v>
-      </c>
-      <c r="J58" t="s">
-        <v>66</v>
+        <v>1885340</v>
+      </c>
+      <c r="J58" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -2339,27 +2280,27 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H59">
-        <v>1857209</v>
-      </c>
-      <c r="J59" t="s">
-        <v>27</v>
+        <v>1885340</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D60">
-        <v>666008</v>
+        <v>661796</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -2368,27 +2309,27 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H60">
-        <v>1857209</v>
+        <v>1885340</v>
       </c>
       <c r="J60" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>42248.845972222225</v>
+        <v>42108</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D61">
-        <v>666008</v>
+        <v>651413</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -2397,213 +2338,201 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H61">
-        <v>1857209</v>
-      </c>
-      <c r="J61" t="b">
-        <v>0</v>
+        <v>1885339</v>
+      </c>
+      <c r="J61">
+        <v>1885339</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>42248.591053240743</v>
+        <v>42108</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D62">
-        <v>657082</v>
+        <v>651413</v>
       </c>
       <c r="E62" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H62">
-        <v>1856386</v>
-      </c>
-      <c r="I62" t="s">
-        <v>68</v>
+        <v>1885339</v>
       </c>
       <c r="J62" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>42248.591053240743</v>
+        <v>42108</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D63">
-        <v>657082</v>
+        <v>651413</v>
       </c>
       <c r="E63" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F63" t="s">
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H63">
-        <v>1856386</v>
+        <v>1885339</v>
       </c>
       <c r="J63" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>42248.576701388891</v>
+        <v>42108</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D64">
-        <v>659339</v>
+        <v>651413</v>
       </c>
       <c r="E64" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F64" t="s">
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H64">
-        <v>1857047</v>
-      </c>
-      <c r="I64" t="s">
-        <v>73</v>
+        <v>1885339</v>
       </c>
       <c r="J64" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>42248.576701388891</v>
+        <v>42108</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D65">
-        <v>659339</v>
+        <v>651413</v>
       </c>
       <c r="E65" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H65">
-        <v>1857047</v>
-      </c>
-      <c r="J65" t="s">
-        <v>75</v>
+        <v>1885339</v>
+      </c>
+      <c r="J65">
+        <v>651413</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>42248.576701388891</v>
+        <v>42108</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D66">
-        <v>659339</v>
+        <v>651413</v>
       </c>
       <c r="E66" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
       </c>
       <c r="G66" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H66">
-        <v>1857047</v>
-      </c>
-      <c r="I66" t="s">
-        <v>29</v>
+        <v>1885339</v>
       </c>
       <c r="J66" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>42248.576701388891</v>
+        <v>42108</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D67">
-        <v>659339</v>
+        <v>651413</v>
       </c>
       <c r="E67" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F67" t="s">
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H67">
-        <v>1857047</v>
-      </c>
-      <c r="I67" t="s">
-        <v>44</v>
+        <v>1885339</v>
       </c>
       <c r="J67" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B68" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D68">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -2615,24 +2544,24 @@
         <v>14</v>
       </c>
       <c r="H68">
-        <v>1857144</v>
-      </c>
-      <c r="J68">
-        <v>1857144</v>
+        <v>1885339</v>
+      </c>
+      <c r="J68" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D69">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
@@ -2641,27 +2570,27 @@
         <v>13</v>
       </c>
       <c r="G69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H69">
-        <v>1857144</v>
-      </c>
-      <c r="J69" t="s">
-        <v>77</v>
+        <v>1885339</v>
+      </c>
+      <c r="J69" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D70">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
@@ -2673,24 +2602,24 @@
         <v>17</v>
       </c>
       <c r="H70">
-        <v>1857144</v>
+        <v>1885339</v>
       </c>
       <c r="J70" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D71">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
@@ -2699,27 +2628,27 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H71">
-        <v>1857144</v>
-      </c>
-      <c r="J71" t="s">
-        <v>35</v>
+        <v>1885339</v>
+      </c>
+      <c r="J71" s="2">
+        <v>42106.327870370369</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D72">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E72" t="s">
         <v>12</v>
@@ -2728,27 +2657,27 @@
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H72">
-        <v>1857144</v>
-      </c>
-      <c r="J72" t="s">
-        <v>63</v>
+        <v>1885339</v>
+      </c>
+      <c r="J72" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D73">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E73" t="s">
         <v>12</v>
@@ -2757,27 +2686,27 @@
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H73">
-        <v>1857144</v>
-      </c>
-      <c r="J73" t="s">
-        <v>27</v>
+        <v>1885339</v>
+      </c>
+      <c r="J73" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D74">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E74" t="s">
         <v>12</v>
@@ -2786,27 +2715,27 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="H74">
-        <v>1857144</v>
-      </c>
-      <c r="J74" t="s">
-        <v>37</v>
+        <v>1885339</v>
+      </c>
+      <c r="J74">
+        <v>133899229</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>42248.076319444444</v>
+        <v>42108</v>
       </c>
       <c r="B75" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D75">
-        <v>613245</v>
+        <v>651413</v>
       </c>
       <c r="E75" t="s">
         <v>12</v>
@@ -2815,178 +2744,172 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H75">
-        <v>1857144</v>
-      </c>
-      <c r="J75" t="b">
-        <v>0</v>
+        <v>1885338</v>
+      </c>
+      <c r="J75">
+        <v>1885338</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>42248.811574074076</v>
+        <v>42108</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D76">
-        <v>663585</v>
+        <v>651413</v>
       </c>
       <c r="E76" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H76">
-        <v>1857078</v>
-      </c>
-      <c r="I76" t="s">
-        <v>78</v>
+        <v>1885338</v>
       </c>
       <c r="J76" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>42248.811574074076</v>
+        <v>42108</v>
       </c>
       <c r="B77" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D77">
-        <v>663585</v>
+        <v>651413</v>
       </c>
       <c r="E77" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F77" t="s">
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H77">
-        <v>1857078</v>
-      </c>
-      <c r="I77" t="s">
-        <v>80</v>
+        <v>1885338</v>
       </c>
       <c r="J77" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>42248.811574074076</v>
+        <v>42108</v>
       </c>
       <c r="B78" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C78" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D78">
-        <v>663585</v>
+        <v>651413</v>
       </c>
       <c r="E78" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F78" t="s">
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H78">
-        <v>1857078</v>
+        <v>1885338</v>
       </c>
       <c r="J78" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>42248.811574074076</v>
+        <v>42108</v>
       </c>
       <c r="B79" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D79">
-        <v>663585</v>
+        <v>651413</v>
       </c>
       <c r="E79" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F79" t="s">
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H79">
-        <v>1857078</v>
-      </c>
-      <c r="J79" t="s">
-        <v>48</v>
+        <v>1885338</v>
+      </c>
+      <c r="J79">
+        <v>651413</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>42248.811574074076</v>
+        <v>42108</v>
       </c>
       <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80">
+        <v>661793</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="s">
+        <v>13</v>
+      </c>
+      <c r="G80" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80">
+        <v>1885333</v>
+      </c>
+      <c r="J80" t="s">
         <v>45</v>
-      </c>
-      <c r="C80" t="s">
-        <v>39</v>
-      </c>
-      <c r="D80">
-        <v>663585</v>
-      </c>
-      <c r="E80" t="s">
-        <v>40</v>
-      </c>
-      <c r="F80" t="s">
-        <v>13</v>
-      </c>
-      <c r="G80" t="s">
-        <v>30</v>
-      </c>
-      <c r="H80">
-        <v>1857078</v>
-      </c>
-      <c r="J80">
-        <v>702912</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B81" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D81">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E81" t="s">
         <v>12</v>
@@ -2995,27 +2918,27 @@
         <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H81">
-        <v>1857212</v>
-      </c>
-      <c r="J81">
-        <v>1857212</v>
+        <v>1885333</v>
+      </c>
+      <c r="J81" s="2">
+        <v>42106.002685185187</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D82">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E82" t="s">
         <v>12</v>
@@ -3024,27 +2947,27 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H82">
-        <v>1857212</v>
-      </c>
-      <c r="J82" t="s">
-        <v>82</v>
+        <v>1885333</v>
+      </c>
+      <c r="J82" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B83" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D83">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E83" t="s">
         <v>12</v>
@@ -3053,27 +2976,27 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H83">
-        <v>1857212</v>
-      </c>
-      <c r="J83" t="s">
-        <v>56</v>
+        <v>1885333</v>
+      </c>
+      <c r="J83" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D84">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E84" t="s">
         <v>12</v>
@@ -3082,27 +3005,27 @@
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H84">
-        <v>1857212</v>
+        <v>1885333</v>
       </c>
       <c r="J84" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D85">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E85" t="s">
         <v>12</v>
@@ -3111,27 +3034,27 @@
         <v>13</v>
       </c>
       <c r="G85" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H85">
-        <v>1857212</v>
-      </c>
-      <c r="J85" t="s">
-        <v>66</v>
+        <v>1885332</v>
+      </c>
+      <c r="J85">
+        <v>1885332</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D86">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E86" t="s">
         <v>12</v>
@@ -3143,24 +3066,24 @@
         <v>26</v>
       </c>
       <c r="H86">
-        <v>1857212</v>
+        <v>1885332</v>
       </c>
       <c r="J86" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D87">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E87" t="s">
         <v>12</v>
@@ -3172,24 +3095,24 @@
         <v>28</v>
       </c>
       <c r="H87">
-        <v>1857212</v>
+        <v>1885332</v>
       </c>
       <c r="J87" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>42248.862905092596</v>
+        <v>42108</v>
       </c>
       <c r="B88" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D88">
-        <v>614735</v>
+        <v>661793</v>
       </c>
       <c r="E88" t="s">
         <v>12</v>
@@ -3198,27 +3121,27 @@
         <v>13</v>
       </c>
       <c r="G88" t="s">
+        <v>30</v>
+      </c>
+      <c r="H88">
+        <v>1885332</v>
+      </c>
+      <c r="J88" t="s">
         <v>31</v>
-      </c>
-      <c r="H88">
-        <v>1857212</v>
-      </c>
-      <c r="J88" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D89">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E89" t="s">
         <v>12</v>
@@ -3227,27 +3150,27 @@
         <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H89">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J89">
-        <v>1857201</v>
+        <v>661793</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D90">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E90" t="s">
         <v>12</v>
@@ -3256,27 +3179,27 @@
         <v>13</v>
       </c>
       <c r="G90" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H90">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J90" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B91" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C91" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D91">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E91" t="s">
         <v>12</v>
@@ -3285,27 +3208,27 @@
         <v>13</v>
       </c>
       <c r="G91" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H91">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J91" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D92">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E92" t="s">
         <v>12</v>
@@ -3314,27 +3237,27 @@
         <v>13</v>
       </c>
       <c r="G92" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H92">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J92" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D93">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E93" t="s">
         <v>12</v>
@@ -3343,27 +3266,27 @@
         <v>13</v>
       </c>
       <c r="G93" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H93">
-        <v>1857201</v>
-      </c>
-      <c r="J93" t="s">
-        <v>85</v>
+        <v>1885332</v>
+      </c>
+      <c r="J93" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C94" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D94">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E94" t="s">
         <v>12</v>
@@ -3372,27 +3295,27 @@
         <v>13</v>
       </c>
       <c r="G94" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H94">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J94" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D95">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E95" t="s">
         <v>12</v>
@@ -3401,27 +3324,27 @@
         <v>13</v>
       </c>
       <c r="G95" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H95">
-        <v>1857201</v>
-      </c>
-      <c r="J95" t="s">
-        <v>37</v>
+        <v>1885332</v>
+      </c>
+      <c r="J95" s="2">
+        <v>42106.000011574077</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D96">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E96" t="s">
         <v>12</v>
@@ -3430,27 +3353,27 @@
         <v>13</v>
       </c>
       <c r="G96" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H96">
-        <v>1857201</v>
-      </c>
-      <c r="J96">
-        <v>638046</v>
+        <v>1885332</v>
+      </c>
+      <c r="J96" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>42248.771863425929</v>
+        <v>42108</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D97">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E97" t="s">
         <v>12</v>
@@ -3459,10 +3382,10 @@
         <v>13</v>
       </c>
       <c r="G97" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H97">
-        <v>1857201</v>
+        <v>1885332</v>
       </c>
       <c r="J97" t="b">
         <v>0</v>
@@ -3470,121 +3393,121 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>42248.771689814814</v>
+        <v>42108</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D98">
-        <v>609176</v>
+        <v>661793</v>
       </c>
       <c r="E98" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F98" t="s">
         <v>13</v>
       </c>
       <c r="G98" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H98">
-        <v>1837800</v>
-      </c>
-      <c r="I98" t="s">
-        <v>58</v>
+        <v>1885332</v>
       </c>
       <c r="J98" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>42248.771689814814</v>
+        <v>42108</v>
       </c>
       <c r="B99" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="C99" t="s">
         <v>11</v>
       </c>
       <c r="D99">
-        <v>609176</v>
+        <v>661797</v>
       </c>
       <c r="E99" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="F99" t="s">
         <v>13</v>
       </c>
       <c r="G99" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H99">
-        <v>1837800</v>
-      </c>
-      <c r="J99" t="s">
-        <v>87</v>
+        <v>1850985</v>
+      </c>
+      <c r="I99">
+        <v>623915</v>
+      </c>
+      <c r="J99">
+        <v>661797</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>42248.925694444442</v>
+        <v>42108</v>
       </c>
       <c r="B100" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C100" t="s">
         <v>11</v>
       </c>
       <c r="D100">
-        <v>610017</v>
+        <v>661797</v>
       </c>
       <c r="E100" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="F100" t="s">
         <v>13</v>
       </c>
       <c r="G100" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H100">
-        <v>1857221</v>
-      </c>
-      <c r="J100">
-        <v>1857221</v>
+        <v>1850985</v>
+      </c>
+      <c r="J100" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>42248.925694444442</v>
+        <v>42108</v>
       </c>
       <c r="B101" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
         <v>11</v>
       </c>
       <c r="D101">
-        <v>610017</v>
+        <v>661797</v>
       </c>
       <c r="E101" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="F101" t="s">
         <v>13</v>
       </c>
       <c r="G101" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H101">
-        <v>1857221</v>
+        <v>1850985</v>
       </c>
       <c r="J101" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>